<commit_message>
ADD test cases for Marchenko
</commit_message>
<xml_diff>
--- a/test_case_notepad_Marchenko.xlsx
+++ b/test_case_notepad_Marchenko.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
   <si>
     <t>id</t>
   </si>
@@ -249,9 +249,6 @@
     <t>NTP-009</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre-condition.Enter the text in notepad.Click on edit menu. Click on Go To function. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Some text is displeyed. Edit context menu is displayed. Field "go to line" is displayed. </t>
   </si>
   <si>
@@ -283,6 +280,36 @@
   </si>
   <si>
     <t>Cancels any last action.</t>
+  </si>
+  <si>
+    <t>Delete function verifikation.</t>
+  </si>
+  <si>
+    <t>Find function verifikation.</t>
+  </si>
+  <si>
+    <t>Find Next function verifikation.</t>
+  </si>
+  <si>
+    <t>Edit context menu verifikation. Undo function verification.</t>
+  </si>
+  <si>
+    <t>Go To  function verifikation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-condition.Enter the text in notepad.Click on Edit menu. Click on Go To function. </t>
+  </si>
+  <si>
+    <t>Select All, Time Date, Undo  function verifikation.</t>
+  </si>
+  <si>
+    <t>Reples, Reples all function verifikation.</t>
+  </si>
+  <si>
+    <t>Copy, Paste function verifikation.</t>
+  </si>
+  <si>
+    <t>Edit context menu verifikation. Cut, Paste verification.</t>
   </si>
 </sst>
 </file>
@@ -372,15 +399,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -398,6 +416,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -406,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
@@ -421,14 +454,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -441,6 +471,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -742,43 +778,43 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" activeCellId="18" sqref="A21:XFD21 A22:XFD22 A23:XFD23 A24:XFD24 A25:XFD25 A26:XFD26 A27:XFD27 A28:XFD28 A29:XFD29 A30:XFD30 A31:XFD31 A32:XFD32 A33:XFD33 A34:XFD34 A35:XFD35 A36:XFD36 A37:XFD37 A38:XFD38 A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75">
-      <c r="A2" s="13"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="60">
       <c r="A3" s="2" t="s">
@@ -827,7 +863,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="60">
+    <row r="6" spans="1:8" ht="75">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -835,7 +871,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
@@ -895,7 +931,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="75">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -903,7 +939,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -936,10 +972,10 @@
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G12" s="4"/>
@@ -951,7 +987,7 @@
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="13" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -982,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
@@ -1006,7 +1042,7 @@
       <c r="F16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="8"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="75">
       <c r="A17" s="4"/>
@@ -1031,13 +1067,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G18" s="4"/>
@@ -1080,13 +1116,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G21" s="4"/>
@@ -1144,7 +1180,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
@@ -1163,7 +1199,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
@@ -1287,14 +1323,14 @@
         <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G34" s="4"/>
     </row>
@@ -1306,29 +1342,29 @@
         <v>11</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="75">
       <c r="A36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="G36" s="4"/>
     </row>
@@ -1340,10 +1376,10 @@
         <v>11</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G37" s="4"/>
     </row>
@@ -1355,10 +1391,10 @@
         <v>14</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="G38" s="4"/>
     </row>
@@ -1373,7 +1409,7 @@
         <v>74</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G39" s="4"/>
     </row>

</xml_diff>